<commit_message>
🔧 Fix contact data handling by updating response structure and removing unnecessary logging
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztofpalpuchowski/Documents/GitHub/passive-income/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C45B7-E310-9B42-9B03-C80CB6ABB985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1D7461-9761-D245-B9FC-E784BC171EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34240" yWindow="740" windowWidth="28040" windowHeight="17240" xr2:uid="{C6CD7F38-079A-084A-8AEA-E40BF107E6DC}"/>
   </bookViews>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0700083-65EB-F045-B424-5C48CDBBC4DD}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>